<commit_message>
Non data files after adding dfc.
</commit_message>
<xml_diff>
--- a/Data_Raw/Assistance/DFC investments.xlsx
+++ b/Data_Raw/Assistance/DFC investments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csis365.sharepoint.com/sites/OfficeofStrategicCapital/Shared Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Greg\Repositories\Vendor\Data_Raw\Assistance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="903" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24B6C272-29B2-4136-8C11-6FD7AB00AB1F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33441C96-B317-463D-BD35-F60F8569C616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -95,9 +95,6 @@
     <t>Project</t>
   </si>
   <si>
-    <t>Committment level</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -801,6 +798,9 @@
   </si>
   <si>
     <t>Count of Sector</t>
+  </si>
+  <si>
+    <t>Commitment level</t>
   </si>
 </sst>
 </file>
@@ -4067,7 +4067,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1EA6F507-9390-4534-839D-5E98860755BB}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1EA6F507-9390-4534-839D-5E98860755BB}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -4153,7 +4153,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{77A6F27C-EE4D-4F74-AF2C-7728A6A9D4B1}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{77A6F27C-EE4D-4F74-AF2C-7728A6A9D4B1}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
   <location ref="A2:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -4339,7 +4339,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5A8AFE3D-5056-47D0-88B3-40F47684F9AE}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5A8AFE3D-5056-47D0-88B3-40F47684F9AE}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="5">
   <location ref="C4:D9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
@@ -4896,8 +4896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4927,13 +4927,13 @@
         <v>16</v>
       </c>
       <c r="G1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4944,25 +4944,25 @@
         <v>2012</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
       </c>
       <c r="G2" s="2">
         <v>250000000</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
         <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4973,25 +4973,25 @@
         <v>2016</v>
       </c>
       <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
       </c>
       <c r="G3" s="2">
         <v>99589373</v>
       </c>
       <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
         <v>30</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -5002,25 +5002,25 @@
         <v>2016</v>
       </c>
       <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
       </c>
       <c r="G4" s="3">
         <v>25409553</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5031,25 +5031,25 @@
         <v>2016</v>
       </c>
       <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
         <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
       </c>
       <c r="G5" s="3">
         <v>5212067</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -5060,25 +5060,25 @@
         <v>2016</v>
       </c>
       <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" s="3">
         <v>4601913</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -5089,25 +5089,25 @@
         <v>2016</v>
       </c>
       <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="3">
         <v>3686231</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -5118,25 +5118,25 @@
         <v>2016</v>
       </c>
       <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G8" s="3">
         <v>3150658</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -5147,25 +5147,25 @@
         <v>2016</v>
       </c>
       <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="3">
         <v>3131290</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -5176,25 +5176,25 @@
         <v>2016</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
         <v>46</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" t="s">
-        <v>47</v>
       </c>
       <c r="G10" s="3">
         <v>2493486</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -5205,25 +5205,25 @@
         <v>2016</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" s="3">
         <v>1676785</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -5234,25 +5234,25 @@
         <v>2016</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="3">
         <v>1189409</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -5263,25 +5263,25 @@
         <v>2016</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="G13" s="3">
         <v>1003776</v>
       </c>
       <c r="H13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -5292,25 +5292,25 @@
         <v>2016</v>
       </c>
       <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
         <v>54</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" t="s">
-        <v>55</v>
       </c>
       <c r="G14" s="3">
         <v>28000000</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" t="s">
         <v>56</v>
-      </c>
-      <c r="I14" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -5321,25 +5321,25 @@
         <v>2018</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" t="s">
         <v>58</v>
-      </c>
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" t="s">
-        <v>59</v>
       </c>
       <c r="G15" s="3">
         <v>1464617</v>
       </c>
       <c r="H15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -5350,25 +5350,25 @@
         <v>2019</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" s="3">
         <v>14071625</v>
       </c>
       <c r="H16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -5379,25 +5379,25 @@
         <v>2019</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G17" s="3">
         <v>10115351</v>
       </c>
       <c r="H17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -5408,25 +5408,25 @@
         <v>2019</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G18" s="3">
         <v>4946842</v>
       </c>
       <c r="H18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -5437,25 +5437,25 @@
         <v>2019</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" t="s">
         <v>66</v>
-      </c>
-      <c r="F19" t="s">
-        <v>67</v>
       </c>
       <c r="G19" s="3">
         <v>4500000</v>
       </c>
       <c r="H19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" t="s">
         <v>68</v>
-      </c>
-      <c r="I19" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -5466,25 +5466,25 @@
         <v>2019</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" t="s">
         <v>70</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>71</v>
-      </c>
-      <c r="F20" t="s">
-        <v>72</v>
       </c>
       <c r="G20" s="3">
         <v>50000000</v>
       </c>
       <c r="H20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -5495,25 +5495,25 @@
         <v>2019</v>
       </c>
       <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
         <v>74</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>75</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>76</v>
-      </c>
-      <c r="F21" t="s">
-        <v>77</v>
       </c>
       <c r="G21" s="3">
         <v>10000000</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21" t="s">
         <v>78</v>
-      </c>
-      <c r="I21" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -5524,25 +5524,25 @@
         <v>2021</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" t="s">
         <v>80</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>81</v>
-      </c>
-      <c r="F22" t="s">
-        <v>82</v>
       </c>
       <c r="G22" s="3">
         <v>12000000</v>
       </c>
       <c r="H22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I22" t="s">
         <v>83</v>
-      </c>
-      <c r="I22" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -5553,25 +5553,25 @@
         <v>2021</v>
       </c>
       <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
         <v>32</v>
       </c>
-      <c r="D23" t="s">
-        <v>33</v>
-      </c>
       <c r="E23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G23" s="3">
         <v>5000000</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I23" t="s">
         <v>86</v>
-      </c>
-      <c r="I23" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -5582,25 +5582,25 @@
         <v>2021</v>
       </c>
       <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
         <v>32</v>
       </c>
-      <c r="D24" t="s">
-        <v>33</v>
-      </c>
       <c r="E24" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" t="s">
         <v>88</v>
-      </c>
-      <c r="F24" t="s">
-        <v>89</v>
       </c>
       <c r="G24" s="3">
         <v>10000000</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" t="s">
         <v>90</v>
-      </c>
-      <c r="I24" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -5611,25 +5611,25 @@
         <v>2022</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G25" s="3">
         <v>40000000</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" t="s">
         <v>93</v>
-      </c>
-      <c r="I25" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -5640,25 +5640,25 @@
         <v>2022</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" t="s">
         <v>95</v>
-      </c>
-      <c r="E26" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" t="s">
-        <v>96</v>
       </c>
       <c r="G26" s="3">
         <v>7497812</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" t="s">
         <v>97</v>
-      </c>
-      <c r="I26" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -5669,25 +5669,25 @@
         <v>2022</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G27" s="3">
         <v>5000000</v>
       </c>
       <c r="H27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I27" t="s">
         <v>100</v>
-      </c>
-      <c r="I27" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -5698,25 +5698,25 @@
         <v>2022</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" t="s">
         <v>102</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>103</v>
-      </c>
-      <c r="F28" t="s">
-        <v>104</v>
       </c>
       <c r="G28" s="3">
         <v>200000000</v>
       </c>
       <c r="H28" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -5727,25 +5727,25 @@
         <v>2022</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G29" s="8">
         <v>40000000</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -5756,25 +5756,25 @@
         <v>2023</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" t="s">
         <v>109</v>
-      </c>
-      <c r="E30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" t="s">
-        <v>110</v>
       </c>
       <c r="G30" s="3">
         <v>10000000</v>
       </c>
       <c r="H30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I30" t="s">
         <v>111</v>
-      </c>
-      <c r="I30" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -5785,25 +5785,25 @@
         <v>2022</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G31" s="3">
         <v>20000000</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I31" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5814,25 +5814,25 @@
         <v>2022</v>
       </c>
       <c r="C32" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="E32" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G32" s="10">
         <v>500000000</v>
       </c>
       <c r="H32" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I32" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5843,25 +5843,25 @@
         <v>2022</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="9" t="s">
         <v>119</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>120</v>
       </c>
       <c r="G33" s="10">
         <v>25000000</v>
       </c>
       <c r="H33" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I33" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -5872,25 +5872,25 @@
         <v>2022</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G34" s="3">
         <v>100000000</v>
       </c>
       <c r="H34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34" t="s">
         <v>124</v>
-      </c>
-      <c r="I34" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -5901,25 +5901,25 @@
         <v>2022</v>
       </c>
       <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="s">
         <v>32</v>
       </c>
-      <c r="D35" t="s">
-        <v>33</v>
-      </c>
       <c r="E35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G35" s="3">
         <v>20000000</v>
       </c>
       <c r="H35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I35" t="s">
         <v>127</v>
-      </c>
-      <c r="I35" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -5930,25 +5930,25 @@
         <v>2022</v>
       </c>
       <c r="C36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" t="s">
         <v>129</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" t="s">
         <v>130</v>
-      </c>
-      <c r="E36" t="s">
-        <v>103</v>
-      </c>
-      <c r="F36" t="s">
-        <v>131</v>
       </c>
       <c r="G36" s="3">
         <v>50000000</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -5959,25 +5959,25 @@
         <v>2021</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G37" s="3">
         <v>9491461</v>
       </c>
       <c r="H37" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I37" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -5988,25 +5988,25 @@
         <v>2020</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G38" s="3">
         <v>20000000</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I38" t="s">
         <v>137</v>
-      </c>
-      <c r="I38" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -6017,25 +6017,25 @@
         <v>2020</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D39" t="s">
+        <v>138</v>
+      </c>
+      <c r="E39" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" t="s">
         <v>139</v>
-      </c>
-      <c r="E39" t="s">
-        <v>22</v>
-      </c>
-      <c r="F39" t="s">
-        <v>140</v>
       </c>
       <c r="G39" s="3">
         <v>241000000</v>
       </c>
       <c r="H39" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I39" t="s">
         <v>141</v>
-      </c>
-      <c r="I39" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -6046,25 +6046,25 @@
         <v>2020</v>
       </c>
       <c r="C40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" t="s">
         <v>32</v>
       </c>
-      <c r="D40" t="s">
-        <v>33</v>
-      </c>
       <c r="E40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G40" s="3">
         <v>27300000</v>
       </c>
       <c r="H40" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I40" t="s">
         <v>144</v>
-      </c>
-      <c r="I40" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -6075,25 +6075,25 @@
         <v>2020</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G41" s="3">
         <v>1600000</v>
       </c>
       <c r="H41" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I41" t="s">
         <v>147</v>
-      </c>
-      <c r="I41" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -6104,25 +6104,25 @@
         <v>2020</v>
       </c>
       <c r="C42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" t="s">
         <v>32</v>
       </c>
-      <c r="D42" t="s">
-        <v>33</v>
-      </c>
       <c r="E42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G42" s="3">
         <v>142000000</v>
       </c>
       <c r="H42" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I42" t="s">
         <v>150</v>
-      </c>
-      <c r="I42" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -6133,25 +6133,25 @@
         <v>2020</v>
       </c>
       <c r="C43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" t="s">
         <v>32</v>
       </c>
-      <c r="D43" t="s">
-        <v>33</v>
-      </c>
       <c r="E43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G43" s="3">
         <v>53500000</v>
       </c>
       <c r="H43" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I43" t="s">
         <v>153</v>
-      </c>
-      <c r="I43" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -6162,25 +6162,25 @@
         <v>2020</v>
       </c>
       <c r="C44" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" t="s">
         <v>32</v>
       </c>
-      <c r="D44" t="s">
-        <v>33</v>
-      </c>
       <c r="E44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G44" s="3">
         <v>50000000</v>
       </c>
       <c r="H44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I44" t="s">
         <v>156</v>
-      </c>
-      <c r="I44" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -6191,25 +6191,25 @@
         <v>2019</v>
       </c>
       <c r="C45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D45" t="s">
+        <v>157</v>
+      </c>
+      <c r="E45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" t="s">
         <v>158</v>
-      </c>
-      <c r="E45" t="s">
-        <v>22</v>
-      </c>
-      <c r="F45" t="s">
-        <v>159</v>
       </c>
       <c r="G45" s="3">
         <v>10000000</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I45" t="s">
         <v>160</v>
-      </c>
-      <c r="I45" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -6220,25 +6220,25 @@
         <v>2019</v>
       </c>
       <c r="C46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G46" s="3">
         <v>28400000</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -6249,25 +6249,25 @@
         <v>2019</v>
       </c>
       <c r="C47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G47" s="3">
         <v>2160000</v>
       </c>
       <c r="H47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I47" t="s">
         <v>163</v>
-      </c>
-      <c r="I47" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -6278,25 +6278,25 @@
         <v>2019</v>
       </c>
       <c r="C48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F48" t="s">
         <v>165</v>
-      </c>
-      <c r="F48" t="s">
-        <v>166</v>
       </c>
       <c r="G48" s="3">
         <v>4500000</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -6307,25 +6307,25 @@
         <v>2018</v>
       </c>
       <c r="C49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D49" t="s">
+        <v>167</v>
+      </c>
+      <c r="E49" t="s">
         <v>168</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>169</v>
-      </c>
-      <c r="F49" t="s">
-        <v>170</v>
       </c>
       <c r="G49" s="3">
         <v>10000000</v>
       </c>
       <c r="H49" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I49" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -6336,25 +6336,25 @@
         <v>2018</v>
       </c>
       <c r="C50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G50" s="3">
         <v>22500000</v>
       </c>
       <c r="H50" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I50" t="s">
         <v>174</v>
-      </c>
-      <c r="I50" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -6365,25 +6365,25 @@
         <v>2018</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G51" s="3">
         <v>5000000</v>
       </c>
       <c r="H51" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I51" t="s">
         <v>177</v>
-      </c>
-      <c r="I51" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -6394,25 +6394,25 @@
         <v>2017</v>
       </c>
       <c r="C52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D52" t="s">
+        <v>178</v>
+      </c>
+      <c r="E52" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="E52" t="s">
-        <v>22</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="G52" s="3">
         <v>40000000</v>
       </c>
       <c r="H52" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I52" t="s">
         <v>181</v>
-      </c>
-      <c r="I52" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -6423,25 +6423,25 @@
         <v>2017</v>
       </c>
       <c r="C53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D53" t="s">
+        <v>182</v>
+      </c>
+      <c r="E53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" t="s">
         <v>183</v>
-      </c>
-      <c r="E53" t="s">
-        <v>22</v>
-      </c>
-      <c r="F53" t="s">
-        <v>184</v>
       </c>
       <c r="G53" s="3">
         <v>19900000</v>
       </c>
       <c r="H53" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I53" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -6452,25 +6452,25 @@
         <v>2017</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D54" t="s">
+        <v>186</v>
+      </c>
+      <c r="E54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54" t="s">
         <v>187</v>
-      </c>
-      <c r="E54" t="s">
-        <v>22</v>
-      </c>
-      <c r="F54" t="s">
-        <v>188</v>
       </c>
       <c r="G54" s="3">
         <v>49500000</v>
       </c>
       <c r="H54" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I54" t="s">
         <v>189</v>
-      </c>
-      <c r="I54" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -6481,25 +6481,25 @@
         <v>2017</v>
       </c>
       <c r="C55" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" t="s">
         <v>32</v>
       </c>
-      <c r="D55" t="s">
-        <v>33</v>
-      </c>
       <c r="E55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G55" s="3">
         <v>10000000</v>
       </c>
       <c r="H55" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I55" t="s">
         <v>192</v>
-      </c>
-      <c r="I55" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -6510,25 +6510,25 @@
         <v>2017</v>
       </c>
       <c r="C56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D56" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E56" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F56" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G56" s="3">
         <v>50000000</v>
       </c>
       <c r="H56" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I56" t="s">
         <v>195</v>
-      </c>
-      <c r="I56" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -6539,25 +6539,25 @@
         <v>2016</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E57" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F57" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G57" s="3">
         <v>35000000</v>
       </c>
       <c r="H57" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I57" t="s">
         <v>198</v>
-      </c>
-      <c r="I57" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -6568,25 +6568,25 @@
         <v>2015</v>
       </c>
       <c r="C58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D58" t="s">
+        <v>199</v>
+      </c>
+      <c r="E58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" t="s">
         <v>200</v>
-      </c>
-      <c r="E58" t="s">
-        <v>22</v>
-      </c>
-      <c r="F58" t="s">
-        <v>201</v>
       </c>
       <c r="G58" s="3">
         <v>6500000</v>
       </c>
       <c r="H58" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I58" t="s">
         <v>202</v>
-      </c>
-      <c r="I58" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -6597,25 +6597,25 @@
         <v>2015</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D59" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E59" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F59" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G59" s="3">
         <v>15500000</v>
       </c>
       <c r="H59" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I59" t="s">
         <v>205</v>
-      </c>
-      <c r="I59" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -6626,25 +6626,25 @@
         <v>2015</v>
       </c>
       <c r="C60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G60" s="3">
         <v>15000000</v>
       </c>
       <c r="H60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I60" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="I60" s="6" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -6655,25 +6655,25 @@
         <v>2014</v>
       </c>
       <c r="C61" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D61" t="s">
+        <v>208</v>
+      </c>
+      <c r="E61" t="s">
+        <v>21</v>
+      </c>
+      <c r="F61" t="s">
         <v>209</v>
-      </c>
-      <c r="E61" t="s">
-        <v>22</v>
-      </c>
-      <c r="F61" t="s">
-        <v>210</v>
       </c>
       <c r="G61" s="3">
         <v>250000000</v>
       </c>
       <c r="H61" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I61" t="s">
         <v>211</v>
-      </c>
-      <c r="I61" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -6684,25 +6684,25 @@
         <v>2013</v>
       </c>
       <c r="C62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" t="s">
         <v>26</v>
       </c>
-      <c r="D62" t="s">
-        <v>27</v>
-      </c>
       <c r="E62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F62" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G62" s="3">
         <v>250000000</v>
       </c>
       <c r="H62" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I62" t="s">
         <v>214</v>
-      </c>
-      <c r="I62" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -6713,25 +6713,25 @@
         <v>2013</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D63" t="s">
+        <v>215</v>
+      </c>
+      <c r="E63" t="s">
+        <v>21</v>
+      </c>
+      <c r="F63" t="s">
         <v>216</v>
-      </c>
-      <c r="E63" t="s">
-        <v>22</v>
-      </c>
-      <c r="F63" t="s">
-        <v>217</v>
       </c>
       <c r="G63" s="3">
         <v>155000000</v>
       </c>
       <c r="H63" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I63" t="s">
         <v>218</v>
-      </c>
-      <c r="I63" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -6742,25 +6742,25 @@
         <v>2011</v>
       </c>
       <c r="C64" t="s">
+        <v>219</v>
+      </c>
+      <c r="D64" t="s">
+        <v>32</v>
+      </c>
+      <c r="E64" t="s">
+        <v>21</v>
+      </c>
+      <c r="F64" t="s">
         <v>220</v>
-      </c>
-      <c r="D64" t="s">
-        <v>33</v>
-      </c>
-      <c r="E64" t="s">
-        <v>22</v>
-      </c>
-      <c r="F64" t="s">
-        <v>221</v>
       </c>
       <c r="G64" s="3">
         <v>150000000</v>
       </c>
       <c r="H64" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I64" t="s">
         <v>222</v>
-      </c>
-      <c r="I64" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -6771,25 +6771,25 @@
         <v>2018</v>
       </c>
       <c r="C65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F65" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G65" s="3">
         <v>100000000</v>
       </c>
       <c r="H65" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I65" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="I65" s="6" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -6800,25 +6800,25 @@
         <v>2022</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D66" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F66" s="9" t="s">
         <v>227</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>228</v>
       </c>
       <c r="G66" s="10">
         <v>50000000</v>
       </c>
       <c r="H66" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="I66" s="12" t="s">
         <v>229</v>
-      </c>
-      <c r="I66" s="12" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -6829,25 +6829,25 @@
         <v>2015</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D67" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="E67" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F67" s="18" t="s">
         <v>231</v>
-      </c>
-      <c r="E67" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F67" s="18" t="s">
-        <v>232</v>
       </c>
       <c r="G67" s="19">
         <v>250000000</v>
       </c>
       <c r="H67" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="I67" s="18" t="s">
         <v>233</v>
-      </c>
-      <c r="I67" s="18" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -6858,25 +6858,25 @@
         <v>2023</v>
       </c>
       <c r="C68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" t="s">
         <v>32</v>
       </c>
-      <c r="D68" t="s">
-        <v>33</v>
-      </c>
       <c r="E68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F68" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G68" s="3">
         <v>5000000</v>
       </c>
       <c r="H68" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I68" t="s">
         <v>236</v>
-      </c>
-      <c r="I68" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -6887,25 +6887,25 @@
         <v>2021</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G69" s="10">
         <v>300000000</v>
       </c>
       <c r="H69" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="I69" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="I69" s="12" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -6916,25 +6916,25 @@
         <v>2021</v>
       </c>
       <c r="C70" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E70" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F70" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G70" s="3">
         <v>4500000</v>
       </c>
       <c r="H70" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I70" t="s">
         <v>242</v>
-      </c>
-      <c r="I70" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -6945,25 +6945,25 @@
         <v>2010</v>
       </c>
       <c r="C71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D71" t="s">
+        <v>243</v>
+      </c>
+      <c r="E71" t="s">
+        <v>21</v>
+      </c>
+      <c r="F71" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="E71" t="s">
-        <v>22</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>245</v>
       </c>
       <c r="G71" s="3">
         <v>150000000</v>
       </c>
       <c r="H71" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="I71" t="s">
         <v>246</v>
-      </c>
-      <c r="I71" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -6974,25 +6974,25 @@
         <v>2023</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G72" s="10">
         <v>10000000</v>
       </c>
       <c r="H72" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="I72" s="9" t="s">
         <v>249</v>
-      </c>
-      <c r="I72" s="9" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -7082,7 +7082,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2">
         <v>1237111264</v>
@@ -7090,7 +7090,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2">
         <v>1060209553</v>
@@ -7098,7 +7098,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2">
         <v>527500000</v>
@@ -7106,7 +7106,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B6" s="2">
         <v>450000000</v>
@@ -7114,7 +7114,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2">
         <v>407497812</v>
@@ -7122,7 +7122,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" s="2">
         <v>340000000</v>
@@ -7130,7 +7130,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="2">
         <v>69991461</v>
@@ -7138,7 +7138,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2">
         <v>19782159</v>
@@ -7175,7 +7175,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -7183,7 +7183,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -7233,29 +7233,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="81be2ba9-d44a-427c-bf72-177d1da2197a">
-      <UserInfo>
-        <DisplayName>Greg Sanders</DisplayName>
-        <AccountId>21</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CFBBA41E47174E45A9231C16C01233E1" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c31302cb27e56e4197c5f0e6e0a14a16">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ead9d1e6-6b43-46ca-a195-6f752be8e1c1" xmlns:ns3="81be2ba9-d44a-427c-bf72-177d1da2197a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2eb4c4f3c44300fd461b9af1a041c762" ns2:_="" ns3:_="">
     <xsd:import namespace="ead9d1e6-6b43-46ca-a195-6f752be8e1c1"/>
@@ -7426,25 +7403,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A14A13AE-41BA-451E-9A87-C1EDA73AD746}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="81be2ba9-d44a-427c-bf72-177d1da2197a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E216741C-4825-420B-B57D-27A83E8321FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="81be2ba9-d44a-427c-bf72-177d1da2197a">
+      <UserInfo>
+        <DisplayName>Greg Sanders</DisplayName>
+        <AccountId>21</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6017913-68D3-41AD-95D1-F2A295429D8D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7461,4 +7443,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E216741C-4825-420B-B57D-27A83E8321FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A14A13AE-41BA-451E-9A87-C1EDA73AD746}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="81be2ba9-d44a-427c-bf72-177d1da2197a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>